<commit_message>
Update EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx with new data
</commit_message>
<xml_diff>
--- a/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
+++ b/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dc407a335d7300f/Documentos/GitHub/BusinessSim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="468" documentId="11_300C377E292435E26BC7E9727970CF20457E0EE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C6EFE9A-C269-4793-B1D4-34D3873DD220}"/>
+  <xr:revisionPtr revIDLastSave="497" documentId="11_300C377E292435E26BC7E9727970CF20457E0EE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040BF187-44CC-4C0F-B0E1-D589DF8C14E2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -1075,105 +1075,105 @@
       <b/>
       <sz val="14"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF0000FF"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF008000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF008000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FFFF6B00"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF008000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -1181,27 +1181,27 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF008000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1807,14 +1807,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="7" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2966,7 +2969,7 @@
         <v>7.4205640167003276E+22</v>
       </c>
       <c r="D94" s="22">
-        <f t="shared" si="1"/>
+        <f>B94*C94</f>
         <v>7.4205640167003276E+22</v>
       </c>
       <c r="E94" s="23" t="str">
@@ -3096,14 +3099,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3456,7 +3466,7 @@
       </c>
       <c r="B26">
         <f>Costos!F13</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -3511,7 +3521,7 @@
       </c>
       <c r="D31">
         <f ca="1">$B$26+B31*$B$27+C31*$B$28</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -3529,7 +3539,7 @@
       </c>
       <c r="D32">
         <f t="shared" ref="D32:D95" ca="1" si="3">$B$26+B32*$B$27+C32*$B$28</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3547,7 +3557,7 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3565,7 +3575,7 @@
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -3583,7 +3593,7 @@
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -3601,7 +3611,7 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -3619,7 +3629,7 @@
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -3637,7 +3647,7 @@
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -3655,7 +3665,7 @@
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -3673,7 +3683,7 @@
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -3691,7 +3701,7 @@
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -3709,7 +3719,7 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -3727,7 +3737,7 @@
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3745,7 +3755,7 @@
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -3763,7 +3773,7 @@
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -3781,7 +3791,7 @@
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -3799,7 +3809,7 @@
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -3817,7 +3827,7 @@
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -3835,7 +3845,7 @@
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -3853,7 +3863,7 @@
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -3871,7 +3881,7 @@
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -3889,7 +3899,7 @@
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -3907,7 +3917,7 @@
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -3925,7 +3935,7 @@
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -3943,7 +3953,7 @@
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -3961,7 +3971,7 @@
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -3979,7 +3989,7 @@
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -3997,7 +4007,7 @@
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -4015,7 +4025,7 @@
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -4033,7 +4043,7 @@
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -4051,7 +4061,7 @@
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -4069,7 +4079,7 @@
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -4087,7 +4097,7 @@
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -4105,7 +4115,7 @@
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -4123,7 +4133,7 @@
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -4141,7 +4151,7 @@
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -4159,7 +4169,7 @@
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -4177,7 +4187,7 @@
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -4195,7 +4205,7 @@
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -4213,7 +4223,7 @@
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -4231,7 +4241,7 @@
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -4249,7 +4259,7 @@
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -4267,7 +4277,7 @@
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -4285,7 +4295,7 @@
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -4303,7 +4313,7 @@
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -4321,7 +4331,7 @@
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -4339,7 +4349,7 @@
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -4357,7 +4367,7 @@
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -4375,7 +4385,7 @@
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -4393,7 +4403,7 @@
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -4411,7 +4421,7 @@
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -4429,7 +4439,7 @@
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -4447,7 +4457,7 @@
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -4465,7 +4475,7 @@
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -4483,7 +4493,7 @@
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -4501,7 +4511,7 @@
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -4519,7 +4529,7 @@
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -4537,7 +4547,7 @@
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -4555,7 +4565,7 @@
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -4573,7 +4583,7 @@
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -4591,7 +4601,7 @@
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -4609,7 +4619,7 @@
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -4627,7 +4637,7 @@
       </c>
       <c r="D93">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -4645,7 +4655,7 @@
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -4663,7 +4673,7 @@
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -4681,7 +4691,7 @@
       </c>
       <c r="D96">
         <f t="shared" ref="D96:D130" ca="1" si="7">$B$26+B96*$B$27+C96*$B$28</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -4699,7 +4709,7 @@
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -4717,7 +4727,7 @@
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -4735,7 +4745,7 @@
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -4753,7 +4763,7 @@
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -4771,7 +4781,7 @@
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -4789,7 +4799,7 @@
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -4807,7 +4817,7 @@
       </c>
       <c r="D103">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -4825,7 +4835,7 @@
       </c>
       <c r="D104">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -4843,7 +4853,7 @@
       </c>
       <c r="D105">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -4861,7 +4871,7 @@
       </c>
       <c r="D106">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -4879,7 +4889,7 @@
       </c>
       <c r="D107">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -4897,7 +4907,7 @@
       </c>
       <c r="D108">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -4915,7 +4925,7 @@
       </c>
       <c r="D109">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -4933,7 +4943,7 @@
       </c>
       <c r="D110">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -4951,7 +4961,7 @@
       </c>
       <c r="D111">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -4969,7 +4979,7 @@
       </c>
       <c r="D112">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -4987,7 +4997,7 @@
       </c>
       <c r="D113">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -5005,7 +5015,7 @@
       </c>
       <c r="D114">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -5023,7 +5033,7 @@
       </c>
       <c r="D115">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -5041,7 +5051,7 @@
       </c>
       <c r="D116">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -5059,7 +5069,7 @@
       </c>
       <c r="D117">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -5077,7 +5087,7 @@
       </c>
       <c r="D118">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -5095,7 +5105,7 @@
       </c>
       <c r="D119">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -5113,7 +5123,7 @@
       </c>
       <c r="D120">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -5131,7 +5141,7 @@
       </c>
       <c r="D121">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -5149,7 +5159,7 @@
       </c>
       <c r="D122">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -5167,7 +5177,7 @@
       </c>
       <c r="D123">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -5185,7 +5195,7 @@
       </c>
       <c r="D124">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -5203,7 +5213,7 @@
       </c>
       <c r="D125">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -5221,7 +5231,7 @@
       </c>
       <c r="D126">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -5239,7 +5249,7 @@
       </c>
       <c r="D127">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -5257,7 +5267,7 @@
       </c>
       <c r="D128">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -5275,7 +5285,7 @@
       </c>
       <c r="D129">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -5293,7 +5303,7 @@
       </c>
       <c r="D130">
         <f t="shared" ca="1" si="7"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -5302,7 +5312,7 @@
       </c>
       <c r="D132">
         <f ca="1">AVERAGE(D31:D130)</f>
-        <v>3.5792471470981786E+24</v>
+        <v>1.334266812305747E+24</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -5311,7 +5321,7 @@
       </c>
       <c r="D133">
         <f ca="1">_xlfn.PERCENTILE.INC(D31:D130,0.9)</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
   </sheetData>
@@ -5333,12 +5343,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="10" width="13" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5423,7 +5441,7 @@
       </c>
       <c r="B6" s="36">
         <f>Compras_y_Lotes!H13</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
       <c r="C6" s="45">
         <v>0</v>
@@ -5448,7 +5466,7 @@
       </c>
       <c r="J6" s="37">
         <f>B6</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5539,7 +5557,7 @@
       </c>
       <c r="B9" s="67">
         <f t="shared" ref="B9:J9" si="0">SUM(B6:B8)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
       <c r="C9" s="67">
         <f t="shared" si="0"/>
@@ -5571,7 +5589,7 @@
       </c>
       <c r="J9" s="67">
         <f t="shared" si="0"/>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5918,7 +5936,7 @@
       </c>
       <c r="B26" s="68">
         <f t="shared" ref="B26:J26" si="3">B9+B16+B23</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
       <c r="C26" s="68">
         <f t="shared" si="3"/>
@@ -5950,7 +5968,7 @@
       </c>
       <c r="J26" s="68">
         <f t="shared" si="3"/>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5970,7 +5988,7 @@
       </c>
       <c r="B30" s="69">
         <f>MAX(B26:I26)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>247</v>
@@ -5994,7 +6012,7 @@
       </c>
       <c r="B32" s="69">
         <f>AVERAGE(B26:I26)</f>
-        <v>4.4740589338727245E+23</v>
+        <v>1.6678335153821821E+23</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>251</v>
@@ -6006,7 +6024,7 @@
       </c>
       <c r="B33" s="69">
         <f>STDEV(B26:I26)</f>
-        <v>1.2654549922348287E+24</v>
+        <v>4.7173458305374049E+23</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>253</v>
@@ -6031,14 +6049,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -6588,11 +6609,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -6798,7 +6825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7171,7 +7200,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8084,7 +8115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8214,12 +8247,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="11" width="12" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8310,7 +8354,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="25">
-        <f>Inputs!B23</f>
+        <f>_xlfn.XLOOKUP(A6,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>1</v>
       </c>
       <c r="C6" s="26">
@@ -8355,7 +8399,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="25">
-        <f>Inputs!B24</f>
+        <f>_xlfn.XLOOKUP(A7,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>0.2</v>
       </c>
       <c r="C7" s="26">
@@ -8400,7 +8444,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="25">
-        <f>Inputs!B25</f>
+        <f>_xlfn.XLOOKUP(A8,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>0.01</v>
       </c>
       <c r="C8" s="26">
@@ -8445,7 +8489,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="25">
-        <f>Inputs!B26</f>
+        <f>_xlfn.XLOOKUP(A9,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>8</v>
       </c>
       <c r="C9" s="26">
@@ -8490,7 +8534,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="25">
-        <f>Inputs!B27</f>
+        <f>_xlfn.XLOOKUP(A10,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>0.3</v>
       </c>
       <c r="C10" s="26">
@@ -8535,7 +8579,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="25">
-        <f>Inputs!B28</f>
+        <f>_xlfn.XLOOKUP(A11,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>0.6</v>
       </c>
       <c r="C11" s="26">
@@ -8580,7 +8624,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="25">
-        <f>Inputs!B29</f>
+        <f>_xlfn.XLOOKUP(A12,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>2</v>
       </c>
       <c r="C12" s="26">
@@ -8625,7 +8669,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="25">
-        <f>Inputs!B30</f>
+        <f>_xlfn.XLOOKUP(A13,Inputs!$A$22:$A$30,Inputs!$B$22:$B$30)</f>
         <v>0.75</v>
       </c>
       <c r="C13" s="26">
@@ -8723,12 +8767,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="9" width="12" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8825,7 +8878,7 @@
         <v>101</v>
       </c>
       <c r="B7" s="29">
-        <f>Inputs!B11</f>
+        <f>Multi_Planta!D6</f>
         <v>4512</v>
       </c>
       <c r="C7" s="22">
@@ -9009,7 +9062,7 @@
         <v>101</v>
       </c>
       <c r="B13" s="29">
-        <f>Inputs!B12</f>
+        <f>Multi_Planta!D7</f>
         <v>1058</v>
       </c>
       <c r="C13" s="22">
@@ -9193,7 +9246,7 @@
         <v>101</v>
       </c>
       <c r="B19" s="29">
-        <f>Inputs!B13</f>
+        <f>Multi_Planta!D8</f>
         <v>130</v>
       </c>
       <c r="C19" s="22">
@@ -9377,7 +9430,7 @@
         <v>101</v>
       </c>
       <c r="B25" s="29">
-        <f>Inputs!B14</f>
+        <f>Multi_Planta!D9</f>
         <v>5268</v>
       </c>
       <c r="C25" s="22">
@@ -9561,7 +9614,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="29">
-        <f>Inputs!B15</f>
+        <f>Multi_Planta!D10</f>
         <v>4333</v>
       </c>
       <c r="C31" s="22">
@@ -9745,7 +9798,7 @@
         <v>101</v>
       </c>
       <c r="B37" s="29">
-        <f>Inputs!B16</f>
+        <f>Multi_Planta!D11</f>
         <v>8487</v>
       </c>
       <c r="C37" s="22">
@@ -9929,7 +9982,7 @@
         <v>101</v>
       </c>
       <c r="B43" s="29">
-        <f>Inputs!B17</f>
+        <f>Multi_Planta!D12</f>
         <v>23192</v>
       </c>
       <c r="C43" s="22">
@@ -10113,7 +10166,7 @@
         <v>101</v>
       </c>
       <c r="B49" s="29">
-        <f>Inputs!$B$18</f>
+        <f>Multi_Planta!D13</f>
         <v>6035</v>
       </c>
       <c r="C49" s="22">
@@ -10691,12 +10744,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="11" width="11" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -10815,12 +10878,12 @@
         <v>7.4205640167003298E+20</v>
       </c>
       <c r="G7" s="36">
-        <f>Inputs!B45</f>
-        <v>0</v>
+        <f>_xlfn.XLOOKUP(A7,Inputs!$A$49:$A$54,Inputs!$B$49:$B$54)</f>
+        <v>60</v>
       </c>
       <c r="H7" s="37">
         <f t="shared" ref="H7:H12" si="3">E7*G7</f>
-        <v>0</v>
+        <v>1.484112803340066E+21</v>
       </c>
       <c r="I7" s="23" t="str">
         <f t="shared" ref="I7:I12" si="4">IF(F7&gt;=B7,"OK","INSUFICIENTE")</f>
@@ -10852,7 +10915,7 @@
         <v>5.9364512133602641E+23</v>
       </c>
       <c r="G8" s="36">
-        <f>Inputs!B46</f>
+        <f>_xlfn.XLOOKUP(A8,Inputs!$A$49:$A$54,Inputs!$B$49:$B$54)</f>
         <v>7</v>
       </c>
       <c r="H8" s="37">
@@ -10889,12 +10952,12 @@
         <v>2.2261692050100999E+22</v>
       </c>
       <c r="G9" s="36">
-        <f>Inputs!B47</f>
-        <v>125</v>
+        <f>_xlfn.XLOOKUP(A9,Inputs!$A$49:$A$54,Inputs!$B$49:$B$54)</f>
+        <v>36</v>
       </c>
       <c r="H9" s="37">
         <f t="shared" si="3"/>
-        <v>2.7827115062626248E+24</v>
+        <v>8.0142091380363598E+23</v>
       </c>
       <c r="I9" s="23" t="str">
         <f t="shared" si="4"/>
@@ -10926,12 +10989,12 @@
         <v>4.4523384100201997E+22</v>
       </c>
       <c r="G10" s="36">
-        <f>Inputs!B48</f>
-        <v>330</v>
+        <f>_xlfn.XLOOKUP(A10,Inputs!$A$49:$A$54,Inputs!$B$49:$B$54)</f>
+        <v>24</v>
       </c>
       <c r="H10" s="37">
         <f t="shared" si="3"/>
-        <v>1.469271675306666E+23</v>
+        <v>1.068561218404848E+22</v>
       </c>
       <c r="I10" s="23" t="str">
         <f t="shared" si="4"/>
@@ -10963,12 +11026,12 @@
         <v>1.4841128033400658E+23</v>
       </c>
       <c r="G11" s="36">
-        <f>Inputs!B49</f>
-        <v>60</v>
+        <f>_xlfn.XLOOKUP(A11,Inputs!$A$49:$A$54,Inputs!$B$49:$B$54)</f>
+        <v>30</v>
       </c>
       <c r="H11" s="37">
         <f t="shared" si="3"/>
-        <v>2.9682256066801317E+23</v>
+        <v>1.4841128033400658E+23</v>
       </c>
       <c r="I11" s="23" t="str">
         <f t="shared" si="4"/>
@@ -11000,12 +11063,12 @@
         <v>5.5654230125252459E+22</v>
       </c>
       <c r="G12" s="36">
-        <f>Inputs!B50</f>
-        <v>7</v>
+        <f>_xlfn.XLOOKUP(A12,Inputs!$A$49:$A$54,Inputs!$B$49:$B$54)</f>
+        <v>28</v>
       </c>
       <c r="H12" s="37">
         <f t="shared" si="3"/>
-        <v>6.4929935146127867E+21</v>
+        <v>2.5971974058451147E+22</v>
       </c>
       <c r="I12" s="23" t="str">
         <f t="shared" si="4"/>
@@ -11024,7 +11087,7 @@
       <c r="G13" s="83"/>
       <c r="H13" s="38">
         <f>SUM(H7:H12)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11758,11 +11821,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="15" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -11811,7 +11881,7 @@
       </c>
       <c r="B5" s="36">
         <f>Compras_y_Lotes!H7</f>
-        <v>0</v>
+        <v>1.484112803340066E+21</v>
       </c>
       <c r="C5" s="41">
         <v>1</v>
@@ -11824,7 +11894,7 @@
       </c>
       <c r="F5" s="37">
         <f t="shared" ref="F5:F12" si="0">B5+D5+E5</f>
-        <v>0</v>
+        <v>1.484112803340066E+21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11855,7 +11925,7 @@
       </c>
       <c r="B7" s="36">
         <f>Compras_y_Lotes!H9</f>
-        <v>2.7827115062626248E+24</v>
+        <v>8.0142091380363598E+23</v>
       </c>
       <c r="C7" s="41">
         <v>1</v>
@@ -11868,7 +11938,7 @@
       </c>
       <c r="F7" s="37">
         <f t="shared" si="0"/>
-        <v>2.7827115062626248E+24</v>
+        <v>8.0142091380363598E+23</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11877,7 +11947,7 @@
       </c>
       <c r="B8" s="36">
         <f>Compras_y_Lotes!H10</f>
-        <v>1.469271675306666E+23</v>
+        <v>1.068561218404848E+22</v>
       </c>
       <c r="C8" s="41">
         <v>1</v>
@@ -11890,7 +11960,7 @@
       </c>
       <c r="F8" s="37">
         <f t="shared" si="0"/>
-        <v>1.469271675306666E+23</v>
+        <v>1.068561218404848E+22</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11899,7 +11969,7 @@
       </c>
       <c r="B9" s="36">
         <f>Compras_y_Lotes!H11</f>
-        <v>2.9682256066801317E+23</v>
+        <v>1.4841128033400658E+23</v>
       </c>
       <c r="C9" s="41">
         <v>1</v>
@@ -11912,7 +11982,7 @@
       </c>
       <c r="F9" s="37">
         <f t="shared" si="0"/>
-        <v>2.9682256066801317E+23</v>
+        <v>1.4841128033400658E+23</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11921,7 +11991,7 @@
       </c>
       <c r="B10" s="36">
         <f>Compras_y_Lotes!H12</f>
-        <v>6.4929935146127867E+21</v>
+        <v>2.5971974058451147E+22</v>
       </c>
       <c r="C10" s="41">
         <v>1</v>
@@ -11934,7 +12004,7 @@
       </c>
       <c r="F10" s="37">
         <f t="shared" si="0"/>
-        <v>6.4929935146127867E+21</v>
+        <v>2.5971974058451147E+22</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11993,7 +12063,7 @@
       </c>
       <c r="B13" s="38">
         <f>SUM(B5:B12)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
       <c r="C13" s="44">
         <f>SUM(C5:C12)</f>
@@ -12009,7 +12079,7 @@
       </c>
       <c r="F13" s="38">
         <f>SUM(F5:F12)</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
   </sheetData>
@@ -12026,12 +12096,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="10" width="12" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -12120,7 +12194,7 @@
       </c>
       <c r="B6" s="36">
         <f>Compras_y_Lotes!H13</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
       <c r="C6" s="45">
         <v>0</v>
@@ -12145,7 +12219,7 @@
       </c>
       <c r="J6" s="37">
         <f>SUM(B6:I6)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12220,7 +12294,7 @@
       </c>
       <c r="B9" s="38">
         <f t="shared" ref="B9:I9" si="0">SUM(B6:B8)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
       <c r="C9" s="38">
         <f t="shared" si="0"/>
@@ -12252,7 +12326,7 @@
       </c>
       <c r="J9" s="38">
         <f>SUM(B9:I9)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
   </sheetData>
@@ -12270,12 +12344,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="5" width="18" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -12511,23 +12589,23 @@
       </c>
       <c r="B22" s="37">
         <f>Costos!F13</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
       <c r="C22" s="37">
         <f>Costos!F13</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
       <c r="D22" s="37">
         <f>Costos!F13*0.9</f>
-        <v>3.221322432388362E+24</v>
+        <v>1.2008401310751709E+24</v>
       </c>
       <c r="E22" s="48">
         <f>MIN(B22:D22)</f>
-        <v>3.221322432388362E+24</v>
+        <v>1.2008401310751709E+24</v>
       </c>
       <c r="F22" s="37">
         <f t="shared" ref="F22:F27" si="0">MAX(B22:D22)-MIN(B22:D22)</f>
-        <v>3.5792471470981818E+23</v>
+        <v>1.3342668123057449E+23</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12674,11 +12752,11 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31">
         <f>Costos!F13</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
       <c r="C31">
         <f>Cashflow_Integrado!B30</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -12687,10 +12765,10 @@
       </c>
       <c r="B32">
         <f t="dataTable" ref="B32:C34" dt2D="0" dtr="0" r1="E29"/>
-        <v>1.7120456883020339E+24</v>
+        <v>6.3821402433492687E+23</v>
       </c>
       <c r="C32">
-        <v>1.7120457286506825E+24</v>
+        <v>6.3821406468357528E+23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -12698,10 +12776,10 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
       <c r="C33">
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -12709,10 +12787,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B34">
-        <v>6.9745972263766885E+24</v>
+        <v>2.5999807439340891E+24</v>
       </c>
       <c r="C34">
-        <v>6.9745973364035029E+24</v>
+        <v>2.5999808539609029E+24</v>
       </c>
     </row>
   </sheetData>
@@ -12730,11 +12808,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="13" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -13149,12 +13238,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -13187,7 +13278,7 @@
       </c>
       <c r="B5" s="55">
         <f>Costos!F13</f>
-        <v>3.5792471470981802E+24</v>
+        <v>1.3342668123057454E+24</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -13196,7 +13287,7 @@
       </c>
       <c r="B6" s="55">
         <f>Cashflow_Compras!J9</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -13217,7 +13308,7 @@
       </c>
       <c r="B8" s="55">
         <f>MAX(Cashflow_Compras!B9:I9)</f>
-        <v>3.5792472154219326E+24</v>
+        <v>1.3342668806294978E+24</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx with revised data
</commit_message>
<xml_diff>
--- a/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
+++ b/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="497" documentId="11_300C377E292435E26BC7E9727970CF20457E0EE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040BF187-44CC-4C0F-B0E1-D589DF8C14E2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -1447,11 +1447,11 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1807,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
@@ -1821,49 +1821,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1931,12 +1931,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
@@ -2065,12 +2065,12 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
@@ -2199,12 +2199,12 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
@@ -2351,12 +2351,12 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="76" t="s">
+      <c r="A45" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
@@ -2494,13 +2494,13 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="76" t="s">
+      <c r="A57" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="76"/>
-      <c r="C57" s="76"/>
-      <c r="D57" s="76"/>
-      <c r="E57" s="76"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="78"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="78"/>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
@@ -2559,15 +2559,15 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="76"/>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
-      <c r="G64" s="76"/>
+      <c r="B64" s="78"/>
+      <c r="C64" s="78"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="78"/>
+      <c r="F64" s="78"/>
+      <c r="G64" s="78"/>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
@@ -2658,15 +2658,15 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="76" t="s">
+      <c r="A72" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="B72" s="76"/>
-      <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
-      <c r="E72" s="76"/>
-      <c r="F72" s="76"/>
-      <c r="G72" s="76"/>
+      <c r="B72" s="78"/>
+      <c r="C72" s="78"/>
+      <c r="D72" s="78"/>
+      <c r="E72" s="78"/>
+      <c r="F72" s="78"/>
+      <c r="G72" s="78"/>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
@@ -2757,12 +2757,12 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="76" t="s">
+      <c r="A80" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="76"/>
-      <c r="C80" s="76"/>
-      <c r="D80" s="76"/>
+      <c r="B80" s="78"/>
+      <c r="C80" s="78"/>
+      <c r="D80" s="78"/>
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
@@ -2863,22 +2863,22 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="77" t="s">
+      <c r="A88" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="77"/>
-      <c r="C88" s="77"/>
-      <c r="D88" s="77"/>
-      <c r="E88" s="77"/>
+      <c r="B88" s="79"/>
+      <c r="C88" s="79"/>
+      <c r="D88" s="79"/>
+      <c r="E88" s="79"/>
     </row>
     <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="78" t="s">
+      <c r="A89" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="B89" s="78"/>
-      <c r="C89" s="78"/>
-      <c r="D89" s="78"/>
-      <c r="E89" s="78"/>
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="80"/>
+      <c r="E89" s="80"/>
     </row>
     <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
@@ -3076,11 +3076,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A80:D80"/>
     <mergeCell ref="A88:E88"/>
     <mergeCell ref="A89:E89"/>
@@ -3089,6 +3084,11 @@
     <mergeCell ref="A57:E57"/>
     <mergeCell ref="A64:G64"/>
     <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3145,12 +3145,12 @@
       <c r="J2" s="91"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
@@ -3197,18 +3197,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="78" t="s">
         <v>222</v>
       </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
     </row>
     <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
@@ -3314,16 +3314,16 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
@@ -5360,48 +5360,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="77" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>236</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -5593,18 +5593,18 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="78" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
@@ -5762,18 +5762,18 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="78" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="76"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
@@ -5975,12 +5975,12 @@
       <c r="A27" s="92"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="78" t="s">
         <v>245</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="54" t="s">
@@ -6081,13 +6081,13 @@
       <c r="E2" s="82"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>256</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -6221,13 +6221,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="78" t="s">
         <v>262</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -6407,13 +6407,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="78" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -6623,13 +6623,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -6641,13 +6641,13 @@
       <c r="E2" s="81"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>266</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -6835,14 +6835,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -6855,14 +6855,14 @@
       <c r="F2" s="81"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -7234,16 +7234,16 @@
       <c r="H2" s="81"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>292</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -8115,7 +8115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -8147,15 +8147,15 @@
       <c r="G2" s="81"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -8267,20 +8267,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -8785,19 +8785,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -8830,19 +8830,19 @@
       <c r="K3" s="84"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -9014,19 +9014,19 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="76"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -9198,19 +9198,19 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -9382,19 +9382,19 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="76"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="78"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -9566,19 +9566,19 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="76" t="s">
+      <c r="A29" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="76"/>
-      <c r="K29" s="76"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
@@ -9750,19 +9750,19 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="76"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="76"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="78"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="78"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
@@ -9934,19 +9934,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="76" t="s">
+      <c r="A41" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
-      <c r="K41" s="76"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="78"/>
+      <c r="H41" s="78"/>
+      <c r="I41" s="78"/>
+      <c r="J41" s="78"/>
+      <c r="K41" s="78"/>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
@@ -10118,19 +10118,19 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="76" t="s">
+      <c r="A47" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="76"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="76"/>
-      <c r="G47" s="76"/>
-      <c r="H47" s="76"/>
-      <c r="I47" s="76"/>
-      <c r="J47" s="76"/>
-      <c r="K47" s="76"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="78"/>
+      <c r="H47" s="78"/>
+      <c r="I47" s="78"/>
+      <c r="J47" s="78"/>
+      <c r="K47" s="78"/>
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
@@ -10302,18 +10302,18 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="77" t="s">
+      <c r="A53" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="77"/>
-      <c r="C53" s="77"/>
-      <c r="D53" s="77"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="77"/>
-      <c r="G53" s="77"/>
-      <c r="H53" s="77"/>
-      <c r="I53" s="77"/>
-      <c r="J53" s="77"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="79"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
@@ -10677,11 +10677,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A11:K11"/>
     <mergeCell ref="A47:K47"/>
     <mergeCell ref="A53:J53"/>
     <mergeCell ref="A17:K17"/>
@@ -10689,6 +10684,11 @@
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A35:K35"/>
     <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A11:K11"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:I10">
     <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
@@ -10763,20 +10763,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -10811,18 +10811,18 @@
       <c r="L3" s="86"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
     </row>
     <row r="6" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
@@ -11091,20 +11091,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
     </row>
     <row r="17" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -11836,14 +11836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12109,20 +12109,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12357,14 +12357,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12554,14 +12554,14 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
@@ -12827,18 +12827,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12855,18 +12855,18 @@
       <c r="J2" s="81"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -13039,18 +13039,18 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="78" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -13261,16 +13261,16 @@
       <c r="H1" s="87"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="78" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
@@ -13337,16 +13337,16 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="54" t="s">

</xml_diff>

<commit_message>
Update EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx with updated data
</commit_message>
<xml_diff>
--- a/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
+++ b/EXSIM_Mezquite_Purchasing_CORREGIDO.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="497" documentId="11_300C377E292435E26BC7E9727970CF20457E0EE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040BF187-44CC-4C0F-B0E1-D589DF8C14E2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -1447,11 +1447,11 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1807,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1821,49 +1821,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="A1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1931,12 +1931,12 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
@@ -2065,12 +2065,12 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
@@ -2199,12 +2199,12 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="78" t="s">
+      <c r="A33" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
@@ -2351,12 +2351,12 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="78" t="s">
+      <c r="A45" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="78"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
@@ -2494,13 +2494,13 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="78" t="s">
+      <c r="A57" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="78"/>
-      <c r="C57" s="78"/>
-      <c r="D57" s="78"/>
-      <c r="E57" s="78"/>
+      <c r="B57" s="76"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
@@ -2559,15 +2559,15 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="78" t="s">
+      <c r="A64" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="78"/>
-      <c r="C64" s="78"/>
-      <c r="D64" s="78"/>
-      <c r="E64" s="78"/>
-      <c r="F64" s="78"/>
-      <c r="G64" s="78"/>
+      <c r="B64" s="76"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="76"/>
+      <c r="G64" s="76"/>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
@@ -2658,15 +2658,15 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="78" t="s">
+      <c r="A72" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="B72" s="78"/>
-      <c r="C72" s="78"/>
-      <c r="D72" s="78"/>
-      <c r="E72" s="78"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
+      <c r="B72" s="76"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
@@ -2757,12 +2757,12 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="78" t="s">
+      <c r="A80" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="78"/>
-      <c r="C80" s="78"/>
-      <c r="D80" s="78"/>
+      <c r="B80" s="76"/>
+      <c r="C80" s="76"/>
+      <c r="D80" s="76"/>
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
@@ -2863,22 +2863,22 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="79" t="s">
+      <c r="A88" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="79"/>
-      <c r="C88" s="79"/>
-      <c r="D88" s="79"/>
-      <c r="E88" s="79"/>
+      <c r="B88" s="77"/>
+      <c r="C88" s="77"/>
+      <c r="D88" s="77"/>
+      <c r="E88" s="77"/>
     </row>
     <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="80" t="s">
+      <c r="A89" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="B89" s="80"/>
-      <c r="C89" s="80"/>
-      <c r="D89" s="80"/>
-      <c r="E89" s="80"/>
+      <c r="B89" s="78"/>
+      <c r="C89" s="78"/>
+      <c r="D89" s="78"/>
+      <c r="E89" s="78"/>
     </row>
     <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
@@ -3076,6 +3076,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A80:D80"/>
     <mergeCell ref="A88:E88"/>
     <mergeCell ref="A89:E89"/>
@@ -3084,11 +3089,6 @@
     <mergeCell ref="A57:E57"/>
     <mergeCell ref="A64:G64"/>
     <mergeCell ref="A72:G72"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3145,12 +3145,12 @@
       <c r="J2" s="91"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>214</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
@@ -3197,18 +3197,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
     </row>
     <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
@@ -3314,16 +3314,16 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="76" t="s">
         <v>230</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
@@ -5360,48 +5360,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="80" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>236</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -5593,18 +5593,18 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="76" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
@@ -5762,18 +5762,18 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="76" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
@@ -5975,12 +5975,12 @@
       <c r="A27" s="92"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="76" t="s">
         <v>245</v>
       </c>
-      <c r="B28" s="78"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="54" t="s">
@@ -6081,13 +6081,13 @@
       <c r="E2" s="82"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>256</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -6221,13 +6221,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="76" t="s">
         <v>262</v>
       </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -6407,13 +6407,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="76" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -6623,13 +6623,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -6641,13 +6641,13 @@
       <c r="E2" s="81"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -6835,14 +6835,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -6855,14 +6855,14 @@
       <c r="F2" s="81"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -7234,16 +7234,16 @@
       <c r="H2" s="81"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>292</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -8147,15 +8147,15 @@
       <c r="G2" s="81"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
@@ -8267,20 +8267,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -8785,19 +8785,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -8830,19 +8830,19 @@
       <c r="K3" s="84"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -9014,19 +9014,19 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -9198,19 +9198,19 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="78"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -9382,19 +9382,19 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="76"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -9566,19 +9566,19 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="76"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
@@ -9750,19 +9750,19 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="78"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="76"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
@@ -9934,19 +9934,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="78" t="s">
+      <c r="A41" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="78"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
@@ -10118,19 +10118,19 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="78" t="s">
+      <c r="A47" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="78"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="78"/>
-      <c r="G47" s="78"/>
-      <c r="H47" s="78"/>
-      <c r="I47" s="78"/>
-      <c r="J47" s="78"/>
-      <c r="K47" s="78"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
@@ -10302,18 +10302,18 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="79" t="s">
+      <c r="A53" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="77"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="77"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="77"/>
+      <c r="I53" s="77"/>
+      <c r="J53" s="77"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
@@ -10677,6 +10677,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A11:K11"/>
     <mergeCell ref="A47:K47"/>
     <mergeCell ref="A53:J53"/>
     <mergeCell ref="A17:K17"/>
@@ -10684,11 +10689,6 @@
     <mergeCell ref="A29:K29"/>
     <mergeCell ref="A35:K35"/>
     <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A11:K11"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:I10">
     <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
@@ -10744,7 +10744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -10763,20 +10763,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -10811,18 +10811,18 @@
       <c r="L3" s="86"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
     </row>
     <row r="6" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
@@ -11091,20 +11091,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
     </row>
     <row r="17" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -11836,14 +11836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12109,20 +12109,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12357,14 +12357,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12554,14 +12554,14 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
@@ -12827,18 +12827,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
@@ -12855,18 +12855,18 @@
       <c r="J2" s="81"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -13039,18 +13039,18 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="76" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -13261,16 +13261,16 @@
       <c r="H1" s="87"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="76" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
@@ -13337,16 +13337,16 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="76" t="s">
         <v>204</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="54" t="s">

</xml_diff>